<commit_message>
Added wind and solar profiles for W120_S1A and updated scenario for W120_S1A - 120 m HH and one axis tracking
</commit_message>
<xml_diff>
--- a/india_REV_input/Scenarios_Cost_Master.xlsx
+++ b/india_REV_input/Scenarios_Cost_Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="REvalue_input_csv" sheetId="11" r:id="rId1"/>
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="424">
   <si>
     <t>Screening curves</t>
   </si>
@@ -1674,6 +1674,9 @@
   </si>
   <si>
     <t>economic_dispatch_folder_suffix</t>
+  </si>
+  <si>
+    <t>wind120HH_solar1A</t>
   </si>
 </sst>
 </file>
@@ -2092,13 +2095,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="M27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,10 +2118,12 @@
     <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>230</v>
       </c>
@@ -2180,10 +2185,13 @@
         <v>247</v>
       </c>
       <c r="U1" t="s">
+        <v>423</v>
+      </c>
+      <c r="V1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>249</v>
       </c>
@@ -2199,7 +2207,7 @@
         <v>ChcC70m</v>
       </c>
       <c r="E2" s="21" t="str">
-        <f t="shared" ref="E2:U2" si="0">E3</f>
+        <f t="shared" ref="E2:V2" si="0">E3</f>
         <v>ClcC55m</v>
       </c>
       <c r="F2" s="21" t="str">
@@ -2264,15 +2272,19 @@
       </c>
       <c r="U2" s="21" t="str">
         <f t="shared" si="0"/>
+        <v>ClcC70mW120S1A</v>
+      </c>
+      <c r="V2" s="21" t="str">
+        <f t="shared" si="0"/>
         <v>ClcC70mLmod</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>251</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:U3" si="1">CONCATENATE(C10,C13,C15,C17,C19,C23,C27,C30,C33,C36,C38,C41)</f>
+        <f t="shared" ref="C3:V3" si="1">CONCATENATE(C10,C13,C15,C17,C19,C23,C27,C30,C33,C36,C38,C41)</f>
         <v>ClcC70m</v>
       </c>
       <c r="D3" t="str">
@@ -2344,11 +2356,15 @@
         <v>ClcC70mS90d</v>
       </c>
       <c r="U3" t="str">
+        <f t="shared" ref="U3" si="2">CONCATENATE(U10,U13,U15,U17,U19,U23,U27,U30,U33,U36,U38,U41)</f>
+        <v>ClcC70mW120S1A</v>
+      </c>
+      <c r="V3" t="str">
         <f t="shared" si="1"/>
         <v>ClcC70mLmod</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>422</v>
       </c>
@@ -2357,322 +2373,338 @@
         <v>ClcC70m</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:U4" si="2">CONCATENATE(D10,D13,D15,D17,D19,D30,D33,D36,D38,D41)</f>
+        <f t="shared" ref="D4:V4" si="3">CONCATENATE(D10,D13,D15,D17,D19,D30,D33,D36,D38,D41)</f>
         <v>ChcC70m</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC55m</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mH-25</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mH25</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mN64</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mB15</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mB30</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70m</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mW120</v>
       </c>
       <c r="S4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mS1A</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>ClcC70mS90d</v>
       </c>
       <c r="U4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="U4" si="4">CONCATENATE(U10,U13,U15,U17,U19,U30,U33,U36,U38,U41)</f>
+        <v>ClcC70mW120S1A</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="3"/>
         <v>ClcC70mLmod</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>252</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ref="C5:U5" si="3">CONCATENATE(C11,C15,C17,C19,C30,C33,C36,C38,C41)</f>
+        <f t="shared" ref="C5:V5" si="5">CONCATENATE(C11,C15,C17,C19,C30,C33,C36,C38,C41)</f>
         <v>coallc</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coalhc</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcH-25</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcH25</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcN64</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcB15</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcB30</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallc</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcW120</v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcS1A</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>coallcS90d</v>
       </c>
       <c r="U5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="U5" si="6">CONCATENATE(U11,U15,U17,U19,U30,U33,U36,U38,U41)</f>
+        <v>coallcW120S1A</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="5"/>
         <v>coallcLmod</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>253</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:U6" si="4">CONCATENATE(C11,C15,C17,C19,C30,C33,C36,C38,C41)</f>
+        <f t="shared" ref="C6:V6" si="7">CONCATENATE(C11,C15,C17,C19,C30,C33,C36,C38,C41)</f>
         <v>coallc</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coalhc</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcH-25</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcH25</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcN64</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcB15</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcB30</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallc</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcW120</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcS1A</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>coallcS90d</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="U6" si="8">CONCATENATE(U11,U15,U17,U19,U30,U33,U36,U38,U41)</f>
+        <v>coallcW120S1A</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="7"/>
         <v>coallcLmod</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>254</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" ref="C7:U7" si="5">CONCATENATE(C31,"_",C34)</f>
+        <f t="shared" ref="C7:V7" si="9">CONCATENATE(C31,"_",C34)</f>
         <v>W80_S0d</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W120_S0d</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S1A</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>W80_S90d</v>
       </c>
       <c r="U7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="U7" si="10">CONCATENATE(U31,"_",U34)</f>
+        <v>W120_S1A</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="9"/>
         <v>W80_S0d</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>255</v>
       </c>
@@ -2681,79 +2713,83 @@
         <v>coallc</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ref="D8:U8" si="6">CONCATENATE(D11,D23,D27)</f>
+        <f t="shared" ref="D8:V8" si="11">CONCATENATE(D11,D23,D27)</f>
         <v>coalhc</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcW10lc</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcW20lc</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcW30lc</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcS10lc</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcS20lc</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcS30lc</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallcW30lcS30lc</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>coallc</v>
       </c>
       <c r="U8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="U8" si="12">CONCATENATE(U11,U23,U27)</f>
         <v>coallc</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" t="str">
+        <f t="shared" si="11"/>
+        <v>coallc</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>256</v>
       </c>
@@ -2817,8 +2853,11 @@
       <c r="U9" s="21" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>260</v>
       </c>
@@ -2827,160 +2866,168 @@
         <v>Clc</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:U10" si="7">CONCATENATE("C", LEFT(D9,1), "c")</f>
+        <f t="shared" ref="D10:V10" si="13">CONCATENATE("C", LEFT(D9,1), "c")</f>
         <v>Chc</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>Clc</v>
       </c>
       <c r="U10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="U10" si="14">CONCATENATE("C", LEFT(U9,1), "c")</f>
         <v>Clc</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" t="str">
+        <f t="shared" si="13"/>
+        <v>Clc</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>261</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ref="C11:U11" si="8">CONCATENATE("coal",LEFT(C9,1), "c")</f>
+        <f t="shared" ref="C11:V11" si="15">CONCATENATE("coal",LEFT(C9,1), "c")</f>
         <v>coallc</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coalhc</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>coallc</v>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="U11" si="16">CONCATENATE("coal",LEFT(U9,1), "c")</f>
         <v>coallc</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" t="str">
+        <f t="shared" si="15"/>
+        <v>coallc</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>262</v>
       </c>
@@ -3044,8 +3091,11 @@
       <c r="U12" s="21">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" s="21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>264</v>
       </c>
@@ -3054,79 +3104,83 @@
         <v>C70m</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13:U13" si="9">CONCATENATE("C",D12,"m")</f>
+        <f t="shared" ref="D13:V13" si="17">CONCATENATE("C",D12,"m")</f>
         <v>C70m</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C55m</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>C70m</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="U13" si="18">CONCATENATE("C",U12,"m")</f>
         <v>C70m</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" t="str">
+        <f t="shared" si="17"/>
+        <v>C70m</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>265</v>
       </c>
@@ -3190,89 +3244,96 @@
       <c r="U14" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>267</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" ref="C15:U15" si="10">IF(C14=0,"",CONCATENATE("H",C14))</f>
+        <f t="shared" ref="C15:V15" si="19">IF(C14=0,"",CONCATENATE("H",C14))</f>
         <v/>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>H-25</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>H25</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U15" si="20">IF(U14=0,"",CONCATENATE("H",U14))</f>
+        <v/>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>268</v>
       </c>
@@ -3336,89 +3397,96 @@
       <c r="U16" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>270</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C17:U17" si="11">IF(C16=0,"",CONCATENATE("N",C16))</f>
+        <f t="shared" ref="C17:V17" si="21">IF(C16=0,"",CONCATENATE("N",C16))</f>
         <v/>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>N64</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U17" si="22">IF(U16=0,"",CONCATENATE("N",U16))</f>
+        <v/>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>271</v>
       </c>
@@ -3482,170 +3550,181 @@
       <c r="U18" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>273</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" ref="C19:U19" si="12">IF(C18=0,"",CONCATENATE("B",C18))</f>
+        <f t="shared" ref="C19:V19" si="23">IF(C18=0,"",CONCATENATE("B",C18))</f>
         <v/>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v>B15</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v>B30</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U19" si="24">IF(U18=0,"",CONCATENATE("B",U18))</f>
+        <v/>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>274</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" ref="C20:U20" si="13">CONCATENATE("bat", C18)</f>
+        <f t="shared" ref="C20:V20" si="25">CONCATENATE("bat", C18)</f>
         <v>bat0</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat15</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat30</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>bat0</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="U20" si="26">CONCATENATE("bat", U18)</f>
         <v>bat0</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" t="str">
+        <f t="shared" si="25"/>
+        <v>bat0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>275</v>
       </c>
@@ -3709,8 +3788,11 @@
       <c r="U21" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>277</v>
       </c>
@@ -3774,170 +3856,181 @@
       <c r="U22" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>279</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" ref="C23:U23" si="14">IF(C21=0,"",CONCATENATE("W",C21,LEFT(C22,1),"c"))</f>
+        <f t="shared" ref="C23:V23" si="27">IF(C21=0,"",CONCATENATE("W",C21,LEFT(C22,1),"c"))</f>
         <v/>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>W10lc</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>W20lc</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>W30lc</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>W30lc</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U23" si="28">IF(U21=0,"",CONCATENATE("W",U21,LEFT(U22,1),"c"))</f>
+        <v/>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>280</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" ref="C24:U24" si="15">CONCATENATE("wind",UPPER(LEFT(C22,1)), "C",C21)</f>
+        <f t="shared" ref="C24:V24" si="29">CONCATENATE("wind",UPPER(LEFT(C22,1)), "C",C21)</f>
         <v>windLC0</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC10</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC20</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC30</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC30</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>windLC0</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="U24" si="30">CONCATENATE("wind",UPPER(LEFT(U22,1)), "C",U21)</f>
         <v>windLC0</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" t="str">
+        <f t="shared" si="29"/>
+        <v>windLC0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>281</v>
       </c>
@@ -4001,8 +4094,11 @@
       <c r="U25" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>282</v>
       </c>
@@ -4066,170 +4162,181 @@
       <c r="U26" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>283</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" ref="C27:M27" si="16">IF(C25=0,"",CONCATENATE("W",C25,LEFT(C26,1),"c"))</f>
+        <f t="shared" ref="C27:M27" si="31">IF(C25=0,"",CONCATENATE("W",C25,LEFT(C26,1),"c"))</f>
         <v/>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="N27" t="str">
-        <f t="shared" ref="N27:U27" si="17">IF(N25=0,"",CONCATENATE("S",N25,LEFT(N26,1),"c"))</f>
+        <f t="shared" ref="N27:V27" si="32">IF(N25=0,"",CONCATENATE("S",N25,LEFT(N26,1),"c"))</f>
         <v>S10lc</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>S20lc</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>S30lc</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>S30lc</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U27" si="33">IF(U25=0,"",CONCATENATE("S",U25,LEFT(U26,1),"c"))</f>
+        <v/>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>284</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" ref="C28:U28" si="18">CONCATENATE("solar",UPPER(LEFT(C26,1)), "C",C25)</f>
+        <f t="shared" ref="C28:V28" si="34">CONCATENATE("solar",UPPER(LEFT(C26,1)), "C",C25)</f>
         <v>solarLC0</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC10</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC20</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC30</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC30</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="34"/>
         <v>solarLC0</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="U28" si="35">CONCATENATE("solar",UPPER(LEFT(U26,1)), "C",U25)</f>
         <v>solarLC0</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" t="str">
+        <f t="shared" si="34"/>
+        <v>solarLC0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>285</v>
       </c>
@@ -4291,172 +4398,183 @@
         <v>80</v>
       </c>
       <c r="U29" s="21">
+        <v>120</v>
+      </c>
+      <c r="V29" s="21">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>287</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" ref="C30:U30" si="19">IF(C29=80,"", CONCATENATE("W",C29))</f>
+        <f t="shared" ref="C30:V30" si="36">IF(C29=80,"", CONCATENATE("W",C29))</f>
         <v/>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="O30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>W120</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U30" si="37">IF(U29=80,"", CONCATENATE("W",U29))</f>
+        <v>W120</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>288</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" ref="C31:U31" si="20">CONCATENATE("W",C29)</f>
+        <f t="shared" ref="C31:V31" si="38">CONCATENATE("W",C29)</f>
         <v>W80</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W120</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="U31" si="39">CONCATENATE("W",U29)</f>
+        <v>W120</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="38"/>
         <v>W80</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>289</v>
       </c>
@@ -4518,172 +4636,183 @@
         <v>293</v>
       </c>
       <c r="U32" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="V32" s="21" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>294</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" ref="C33:U33" si="21">IF(C32="0d", "", CONCATENATE("S",C32))</f>
+        <f t="shared" ref="C33:V33" si="40">IF(C32="0d", "", CONCATENATE("S",C32))</f>
         <v/>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v>S1A</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v>S90d</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U33" si="41">IF(U32="0d", "", CONCATENATE("S",U32))</f>
+        <v>S1A</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>295</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" ref="C34:U34" si="22">CONCATENATE("S",C32)</f>
+        <f t="shared" ref="C34:V34" si="42">CONCATENATE("S",C32)</f>
         <v>S0d</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S1A</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>S90d</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="U34" si="43">CONCATENATE("S",U32)</f>
+        <v>S1A</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="42"/>
         <v>S0d</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>296</v>
       </c>
@@ -4745,89 +4874,96 @@
       <c r="U35" s="21">
         <v>2014</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V35" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>297</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36:U36" si="23">IF(C35=2014,"",CONCATENATE("L",C35))</f>
+        <f t="shared" ref="C36:V36" si="44">IF(C35=2014,"",CONCATENATE("L",C35))</f>
         <v/>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U36" si="45">IF(U35=2014,"",CONCATENATE("L",U35))</f>
+        <v/>
+      </c>
+      <c r="V36" t="str">
+        <f t="shared" si="44"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>298</v>
       </c>
@@ -4889,91 +5025,98 @@
         <v>300</v>
       </c>
       <c r="U37" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="V37" s="21" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>302</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" ref="C38:U38" si="24">IF(C37="none","",CONCATENATE("L",C37))</f>
+        <f t="shared" ref="C38:V38" si="46">IF(C37="none","",CONCATENATE("L",C37))</f>
         <v/>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="U38" si="47">IF(U37="none","",CONCATENATE("L",U37))</f>
+        <v/>
+      </c>
+      <c r="V38" t="str">
+        <f t="shared" si="46"/>
         <v>Lmod</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>303</v>
       </c>
@@ -5037,8 +5180,11 @@
       <c r="U39" s="21" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V39" s="21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>306</v>
       </c>
@@ -5099,85 +5245,92 @@
       <c r="U40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" ref="C41:U41" si="25">IF(C39="RT","",CONCATENATE(C39,C40))</f>
+        <f t="shared" ref="C41:V41" si="48">IF(C39="RT","",CONCATENATE(C39,C40))</f>
         <v/>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="U41" si="49">IF(U39="RT","",CONCATENATE(U39,U40))</f>
+        <v/>
+      </c>
+      <c r="V41" t="str">
+        <f t="shared" si="48"/>
         <v/>
       </c>
     </row>

</xml_diff>